<commit_message>
Terminada logica del proyecto
terminada la logica del proyecto, generado javadoc
</commit_message>
<xml_diff>
--- a/PracticaUD1/Recursos.xlsx
+++ b/PracticaUD1/Recursos.xlsx
@@ -4005,10 +4005,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
-    <numFmt numFmtId="166" formatCode="0"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -4108,7 +4107,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4165,18 +4164,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1048576"/>
+  <dimension ref="A1:D1035"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A957" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A937" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D2" activeCellId="0" sqref="D2:D956"/>
+      <selection pane="bottomLeft" activeCell="C953" activeCellId="0" sqref="C953"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1017" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1013" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17800,201 +17799,6 @@
     <row r="1035" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D1035" s="5"/>
     </row>
-    <row r="1036" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1036" s="5"/>
-    </row>
-    <row r="1037" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1037" s="5"/>
-    </row>
-    <row r="1038" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1038" s="5"/>
-    </row>
-    <row r="1039" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1039" s="5"/>
-    </row>
-    <row r="1040" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1040" s="5"/>
-    </row>
-    <row r="1041" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1041" s="5"/>
-    </row>
-    <row r="1042" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1042" s="5"/>
-    </row>
-    <row r="1043" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1043" s="5"/>
-    </row>
-    <row r="1044" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1044" s="5"/>
-    </row>
-    <row r="1045" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1045" s="5"/>
-    </row>
-    <row r="1046" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1046" s="5"/>
-    </row>
-    <row r="1047" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1047" s="5"/>
-    </row>
-    <row r="1048" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1048" s="5"/>
-    </row>
-    <row r="1049" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1049" s="5"/>
-    </row>
-    <row r="1050" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1050" s="5"/>
-    </row>
-    <row r="1051" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1051" s="5"/>
-    </row>
-    <row r="1052" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1052" s="5"/>
-    </row>
-    <row r="1053" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1053" s="5"/>
-    </row>
-    <row r="1054" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1054" s="5"/>
-    </row>
-    <row r="1055" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1055" s="5"/>
-    </row>
-    <row r="1056" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1056" s="5"/>
-    </row>
-    <row r="1057" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1057" s="5"/>
-    </row>
-    <row r="1058" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1058" s="5"/>
-    </row>
-    <row r="1059" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1059" s="5"/>
-    </row>
-    <row r="1060" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1060" s="5"/>
-    </row>
-    <row r="1061" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1061" s="5"/>
-    </row>
-    <row r="1062" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1062" s="5"/>
-    </row>
-    <row r="1063" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1063" s="5"/>
-    </row>
-    <row r="1064" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1064" s="5"/>
-    </row>
-    <row r="1065" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1065" s="5"/>
-    </row>
-    <row r="1066" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1066" s="5"/>
-    </row>
-    <row r="1067" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1067" s="5"/>
-    </row>
-    <row r="1068" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1068" s="5"/>
-    </row>
-    <row r="1069" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1069" s="5"/>
-    </row>
-    <row r="1070" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1070" s="5"/>
-    </row>
-    <row r="1071" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1071" s="5"/>
-    </row>
-    <row r="1072" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1072" s="5"/>
-    </row>
-    <row r="1073" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1073" s="5"/>
-    </row>
-    <row r="1074" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1074" s="5"/>
-    </row>
-    <row r="1075" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1075" s="5"/>
-    </row>
-    <row r="1076" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1076" s="5"/>
-    </row>
-    <row r="1077" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1077" s="5"/>
-    </row>
-    <row r="1078" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1078" s="5"/>
-    </row>
-    <row r="1079" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1079" s="5"/>
-    </row>
-    <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <autoFilter ref="A1:C956"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -18016,10 +17820,10 @@
   <dimension ref="A1:C340"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A304" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A341" activeCellId="1" sqref="D2:D956 A341"/>
+      <selection pane="topLeft" activeCell="A341" activeCellId="0" sqref="A341"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.92"/>

</xml_diff>